<commit_message>
corrected timezone error. added interpolated plot.
</commit_message>
<xml_diff>
--- a/data/14HP09/14HP09_index.xlsx
+++ b/data/14HP09/14HP09_index.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,28 +22,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="415">
   <si>
-    <t xml:space="preserve">Experiment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plant_Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genotype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treatment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repeat</t>
+    <t xml:space="preserve">experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plant_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genotype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">repeat</t>
   </si>
   <si>
     <t xml:space="preserve">14HP09</t>
@@ -1364,20 +1364,20 @@
   <dimension ref="A1:H193"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.76020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.82142857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.89795918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2397959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="14.5816326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added interactive visualisations for leaf profiles and dynamics.
</commit_message>
<xml_diff>
--- a/data/14HP09/14HP09_index.xlsx
+++ b/data/14HP09/14HP09_index.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" state="visible" r:id="rId2"/>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">treatment</t>
   </si>
   <si>
-    <t xml:space="preserve">repeat</t>
+    <t xml:space="preserve">rep</t>
   </si>
   <si>
     <t xml:space="preserve">14HP09</t>
@@ -1364,20 +1364,20 @@
   <dimension ref="A1:H193"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H1"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.89795918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2397959183673"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.19897959183674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9795918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.6785714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.3775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6401,7 +6401,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
updated naming in weight objects
</commit_message>
<xml_diff>
--- a/data/14HP09/14HP09_index.xlsx
+++ b/data/14HP09/14HP09_index.xlsx
@@ -1369,18 +1369,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.19897959183674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9795918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.1785714285714"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.6785714285714"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.1989795918367"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>

</xml_diff>